<commit_message>
Update date in schedule file
</commit_message>
<xml_diff>
--- a/docs/downloadables/09-1324A-A_Advantage2_system2_1_annealing_schedule.xlsx
+++ b/docs/downloadables/09-1324A-A_Advantage2_system2_1_annealing_schedule.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\jpasvolsky\pyenv\ocean_repos\dwave_ocean_sdk_3_10_2\dwave-ocean-sdk\docs\downloadables\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C7334B84-9A62-4191-906C-28D88E5E6B38}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{33587E1A-FFA6-4AF0-8199-A5C39AA8AFE2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4245" yWindow="3360" windowWidth="21600" windowHeight="11235" xr2:uid="{3DC0D9D7-D564-4164-9359-4ADAA3FF89FA}"/>
+    <workbookView xWindow="-23595" yWindow="8385" windowWidth="21600" windowHeight="11220" xr2:uid="{3DC0D9D7-D564-4164-9359-4ADAA3FF89FA}"/>
   </bookViews>
   <sheets>
     <sheet name="About" sheetId="2" r:id="rId1"/>
@@ -1253,7 +1253,7 @@
         <v>22</v>
       </c>
       <c r="D14" s="9">
-        <v>45973</v>
+        <v>45986</v>
       </c>
       <c r="E14" s="4"/>
       <c r="F14" s="4"/>

</xml_diff>